<commit_message>
turn off profanity filter, adjust gui size
</commit_message>
<xml_diff>
--- a/swear_words.xlsx
+++ b/swear_words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\PycharmProjects\daa-bmalgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E893BAEB-D7C7-4698-BDA7-3BE659685ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CDE17F-E391-47A2-8DC3-1A0CA0CEF2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,90 +20,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>amputa</t>
+  </si>
+  <si>
+    <t>anak ka ng puta</t>
+  </si>
+  <si>
+    <t>bobo</t>
+  </si>
+  <si>
+    <t>buwiset</t>
+  </si>
+  <si>
+    <t>gaga</t>
+  </si>
+  <si>
+    <t>gagi</t>
+  </si>
+  <si>
+    <t>gago</t>
+  </si>
+  <si>
+    <t>hinayupak</t>
+  </si>
+  <si>
+    <t>kagaguhan</t>
+  </si>
+  <si>
+    <t>kingina</t>
+  </si>
+  <si>
+    <t>kupal</t>
+  </si>
+  <si>
+    <t>leche</t>
+  </si>
+  <si>
+    <t>lintik</t>
+  </si>
+  <si>
+    <t>pakshet</t>
+  </si>
+  <si>
+    <t>pakyu</t>
+  </si>
+  <si>
+    <t>pucha</t>
+  </si>
+  <si>
+    <t>punyeta</t>
+  </si>
+  <si>
+    <t>puta</t>
+  </si>
+  <si>
+    <t>putangina</t>
+  </si>
+  <si>
+    <t>putragis</t>
+  </si>
+  <si>
+    <t>taena</t>
+  </si>
+  <si>
+    <t>tanga</t>
+  </si>
   <si>
     <t>tangina</t>
   </si>
   <si>
-    <t>gago</t>
+    <t>tarantado</t>
+  </si>
+  <si>
+    <t>ulol</t>
+  </si>
+  <si>
+    <t>ulul</t>
+  </si>
+  <si>
+    <t>ungas</t>
   </si>
   <si>
     <t>swear_words_list</t>
   </si>
   <si>
-    <t>amputa</t>
-  </si>
-  <si>
-    <t>anak ka ng puta</t>
-  </si>
-  <si>
-    <t>bobo</t>
-  </si>
-  <si>
-    <t>buwiset</t>
-  </si>
-  <si>
-    <t>gaga</t>
-  </si>
-  <si>
-    <t>gagi</t>
-  </si>
-  <si>
-    <t>hinayupak</t>
-  </si>
-  <si>
-    <t>kagaguhan</t>
-  </si>
-  <si>
-    <t>kingina</t>
-  </si>
-  <si>
-    <t>kupal</t>
-  </si>
-  <si>
-    <t>leche</t>
-  </si>
-  <si>
-    <t>lintik</t>
-  </si>
-  <si>
-    <t>pakshet</t>
-  </si>
-  <si>
-    <t>pakyu</t>
-  </si>
-  <si>
-    <t>pucha</t>
-  </si>
-  <si>
-    <t>punyeta</t>
-  </si>
-  <si>
-    <t>puta</t>
-  </si>
-  <si>
-    <t>putangina</t>
-  </si>
-  <si>
-    <t>putragis</t>
-  </si>
-  <si>
-    <t>taena</t>
-  </si>
-  <si>
-    <t>tanga</t>
-  </si>
-  <si>
-    <t>tarantado</t>
-  </si>
-  <si>
-    <t>ulol</t>
-  </si>
-  <si>
-    <t>ulul</t>
-  </si>
-  <si>
-    <t>ungas</t>
+    <t>tang ina</t>
+  </si>
+  <si>
+    <t>putang ina</t>
   </si>
 </sst>
 </file>
@@ -146,7 +152,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -450,164 +456,171 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A33" s="1"/>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A34" s="1"/>
     </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A35" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added window to show censored words
</commit_message>
<xml_diff>
--- a/swear_words.xlsx
+++ b/swear_words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\PycharmProjects\daa-bmalgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CDE17F-E391-47A2-8DC3-1A0CA0CEF2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C873A932-1008-4B37-9443-5A1E3FEAB18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:A35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -546,17 +546,17 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
added function to add words, changed excel file
</commit_message>
<xml_diff>
--- a/swear_words.xlsx
+++ b/swear_words.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\PycharmProjects\daa-bmalgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C873A932-1008-4B37-9443-5A1E3FEAB18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5CD470-9500-4787-B0A1-8643E6754707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
+    <t>swear_words_list</t>
+  </si>
+  <si>
     <t>amputa</t>
   </si>
   <si>
@@ -73,12 +76,15 @@
     <t>punyeta</t>
   </si>
   <si>
+    <t>putangina</t>
+  </si>
+  <si>
+    <t>putang ina</t>
+  </si>
+  <si>
     <t>puta</t>
   </si>
   <si>
-    <t>putangina</t>
-  </si>
-  <si>
     <t>putragis</t>
   </si>
   <si>
@@ -91,6 +97,9 @@
     <t>tangina</t>
   </si>
   <si>
+    <t>tang ina</t>
+  </si>
+  <si>
     <t>tarantado</t>
   </si>
   <si>
@@ -101,33 +110,16 @@
   </si>
   <si>
     <t>ungas</t>
-  </si>
-  <si>
-    <t>swear_words_list</t>
-  </si>
-  <si>
-    <t>tang ina</t>
-  </si>
-  <si>
-    <t>putang ina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,21 +142,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -197,7 +184,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -209,7 +196,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -256,6 +243,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -291,6 +295,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,105 +464,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.5">
@@ -551,76 +569,60 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A35" s="1"/>
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>